<commit_message>
chore(quality): pnpm unify + api hardening + legacy leak fixes
</commit_message>
<xml_diff>
--- a/docs/plan/TONIGHT_TASKS.xlsx
+++ b/docs/plan/TONIGHT_TASKS.xlsx
@@ -830,12 +830,12 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>doing</t>
+          <t>done</t>
         </is>
       </c>
       <c r="M5" s="2" t="inlineStr">
         <is>
-          <t>codex run: node-monorepo-skeleton</t>
+          <t>commit 70b8a2f（Node monorepo skeleton + compose + README）已 push main</t>
         </is>
       </c>
       <c r="N5" s="2" t="inlineStr">

</xml_diff>